<commit_message>
Export danh sách thống kê
</commit_message>
<xml_diff>
--- a/public/thongke/ExportDSPhieuNhap.xlsx
+++ b/public/thongke/ExportDSPhieuNhap.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Mã phiếu</t>
   </si>
@@ -38,64 +38,10 @@
     <t>P2209-00001</t>
   </si>
   <si>
-    <t>Phiếu nhập thuốc</t>
-  </si>
-  <si>
-    <t>18-09-2022 00:00:00</t>
-  </si>
-  <si>
-    <t>2.000.000 VND</t>
-  </si>
-  <si>
-    <t>P2209-00002</t>
-  </si>
-  <si>
-    <t>Phiếu xuất tháng 9</t>
-  </si>
-  <si>
-    <t>1.000.000 VND</t>
-  </si>
-  <si>
-    <t>P2209-00004</t>
-  </si>
-  <si>
-    <t>Phiếu nhập tháng 11</t>
-  </si>
-  <si>
-    <t>8.000.000 VND</t>
-  </si>
-  <si>
-    <t>P2209-00005</t>
-  </si>
-  <si>
-    <t>Phiếu xuất 2</t>
-  </si>
-  <si>
-    <t>3.000.000 VND</t>
-  </si>
-  <si>
-    <t>P2209-00006</t>
-  </si>
-  <si>
-    <t>P2209-00009</t>
-  </si>
-  <si>
-    <t>Nhập thuốc mới</t>
-  </si>
-  <si>
-    <t>18-09-2022 23:50:46</t>
-  </si>
-  <si>
-    <t>450.000 VND</t>
-  </si>
-  <si>
-    <t>P2209-00011</t>
-  </si>
-  <si>
-    <t>19-09-2022 00:17:51</t>
-  </si>
-  <si>
-    <t>225.000 VND</t>
+    <t>27-09-2022 00:00:00</t>
+  </si>
+  <si>
+    <t>900.000 VND</t>
   </si>
 </sst>
 </file>
@@ -109,7 +55,7 @@
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
@@ -431,7 +377,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +387,10 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="23" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="9.10" bestFit="true" style="0"/>
     <col min="8" max="8" width="9.10" bestFit="true" style="0"/>
     <col min="9" max="9" width="9.10" bestFit="true" style="0"/>
@@ -455,9 +401,14 @@
     <col min="15" max="15" width="9.10" bestFit="true" style="0"/>
     <col min="16" max="16" width="9.10" bestFit="true" style="0"/>
     <col min="17" max="17" width="9.10" bestFit="true" style="0"/>
+    <col min="18" max="18" width="9.10" bestFit="true" style="0"/>
+    <col min="19" max="19" width="9.10" bestFit="true" style="0"/>
+    <col min="20" max="20" width="9.10" bestFit="true" style="0"/>
+    <col min="21" max="21" width="9.10" bestFit="true" style="0"/>
+    <col min="22" max="22" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,117 +428,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6"/>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8"/>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
UPDATE DB + CHỈNH SỬA
</commit_message>
<xml_diff>
--- a/public/thongke/ExportDSPhieuNhap.xlsx
+++ b/public/thongke/ExportDSPhieuNhap.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Mã phiếu</t>
   </si>
@@ -35,13 +35,16 @@
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>P2209-00001</t>
-  </si>
-  <si>
-    <t>30-09-2022 00:00:00</t>
-  </si>
-  <si>
-    <t>1.400.000 VND</t>
+    <t>P2210-00003</t>
+  </si>
+  <si>
+    <t>Phiếu nhập tháng 10</t>
+  </si>
+  <si>
+    <t>11-10-2022 00:00:00</t>
+  </si>
+  <si>
+    <t>1.100.000 VND</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
   <cols>
     <col min="1" max="1" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="17" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="23" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="23" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="23" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="9.10" bestFit="true" style="0"/>
     <col min="8" max="8" width="9.10" bestFit="true" style="0"/>
     <col min="9" max="9" width="9.10" bestFit="true" style="0"/>
@@ -434,16 +437,16 @@
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>